<commit_message>
Completed my single function version
</commit_message>
<xml_diff>
--- a/CH-185 Replace consecutive X.xlsx
+++ b/CH-185 Replace consecutive X.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B392AF4-AC88-4514-9BC4-2E81B9C7987E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6482A34-5DE4-4AEF-82F1-D0F811DD26FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -231,11 +231,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -273,6 +336,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1722,7 +1800,7 @@
   <dimension ref="B1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1732,6 +1810,7 @@
     <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
@@ -1975,7 +2054,132 @@
       <c r="R11"/>
       <c r="S11"/>
     </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="K12" s="14" t="str" cm="1">
+        <f t="array" ref="K12:L20">_xlfn.LET(
+_xlpm.d, Data4[Date],
+_xlpm.id, Data4[ID],
+_xlpm.p, _xlfn.REGEXREPLACE(_xlpm.id, "X{2,}","X",,1),
+_xlfn.VSTACK(Data4[#Headers],_xlfn.HSTACK(_xlpm.d,_xlpm.p))
+)</f>
+        <v>Date</v>
+      </c>
+      <c r="L12" s="15" t="str">
+        <v>ID</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="K13" s="16">
+        <v>45567</v>
+      </c>
+      <c r="L13" s="17" t="str">
+        <v>XM-X12</v>
+      </c>
+      <c r="N13" t="b" cm="1">
+        <f t="array" ref="N13:O20">K13:L20=Data35[]</f>
+        <v>1</v>
+      </c>
+      <c r="O13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="K14" s="16">
+        <v>45568</v>
+      </c>
+      <c r="L14" s="18" t="str">
+        <v>IXM3X</v>
+      </c>
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="K15" s="16">
+        <v>45569</v>
+      </c>
+      <c r="L15" s="18" t="str">
+        <v>87X</v>
+      </c>
+      <c r="N15" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="K16" s="16">
+        <v>45570</v>
+      </c>
+      <c r="L16" s="18" t="str">
+        <v>X8X9X1</v>
+      </c>
+      <c r="N16" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="11:19" x14ac:dyDescent="0.5">
+      <c r="K17" s="16">
+        <v>45571</v>
+      </c>
+      <c r="L17" s="18" t="str">
+        <v>Xmna</v>
+      </c>
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="11:19" x14ac:dyDescent="0.5">
+      <c r="K18" s="16">
+        <v>45572</v>
+      </c>
+      <c r="L18" s="18" t="str">
+        <v>XFX</v>
+      </c>
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="11:19" x14ac:dyDescent="0.5">
+      <c r="K19" s="16">
+        <v>45573</v>
+      </c>
+      <c r="L19" s="18" t="str">
+        <v>X</v>
+      </c>
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="20" spans="11:19" x14ac:dyDescent="0.5">
+      <c r="K20" s="16">
+        <v>45574</v>
+      </c>
+      <c r="L20" s="18" t="str">
+        <v>R</v>
+      </c>
+      <c r="N20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>

</xml_diff>

<commit_message>
One Alt1. No other alt looked good
</commit_message>
<xml_diff>
--- a/CH-185 Replace consecutive X.xlsx
+++ b/CH-185 Replace consecutive X.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6482A34-5DE4-4AEF-82F1-D0F811DD26FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428A777A-7689-43F6-BFA2-79AE4965D29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$F$2:$G$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$F$2:$G$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$F$2:$G$5</definedName>
   </definedNames>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="19">
   <si>
     <t>Result</t>
   </si>
@@ -118,12 +120,15 @@
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
   </si>
+  <si>
+    <t>Interesting the choice of number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +177,14 @@
       <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -295,10 +308,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,12 +345,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,11 +360,21 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="42">
     <dxf>
       <font>
         <b val="0"/>
@@ -635,6 +653,310 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1241,56 +1563,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}" name="Data" displayName="Data" ref="C2:D10" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}" name="Data" displayName="Data" ref="C2:D10" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="C2:D10" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:D10">
     <sortCondition ref="C3:C10"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E9D2B9E8-BF22-47EC-9F78-4895D7ECD803}" name="Date" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{61DAF857-2A1A-4299-9CB6-0F31870FF38D}" name="ID" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{E9D2B9E8-BF22-47EC-9F78-4895D7ECD803}" name="Date" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{61DAF857-2A1A-4299-9CB6-0F31870FF38D}" name="ID" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0025CE4B-7270-49F6-875C-F810B632926D}" name="Data3" displayName="Data3" ref="F2:G10" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0025CE4B-7270-49F6-875C-F810B632926D}" name="Data3" displayName="Data3" ref="F2:G10" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="F2:G10" xr:uid="{0025CE4B-7270-49F6-875C-F810B632926D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F3:G10">
     <sortCondition ref="F3:F10"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{538B4C89-CBEF-44DC-A82C-40408E305663}" name="Date" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{5EF9A9A5-32C5-4ED5-8393-1499A6C45160}" name="ID" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{538B4C89-CBEF-44DC-A82C-40408E305663}" name="Date" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{5EF9A9A5-32C5-4ED5-8393-1499A6C45160}" name="ID" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{60AF4BDB-65D4-4AF9-BE12-BB34ADA6D5FA}" name="Data4" displayName="Data4" ref="C2:D10" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{60AF4BDB-65D4-4AF9-BE12-BB34ADA6D5FA}" name="Data4" displayName="Data4" ref="C2:D10" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="C2:D10" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:D10">
     <sortCondition ref="C3:C10"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F7106DE6-9804-4AAB-8E26-6C852733B0A5}" name="Date" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{331243EE-7953-441B-AED6-9A2C98CDC53C}" name="ID" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{F7106DE6-9804-4AAB-8E26-6C852733B0A5}" name="Date" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{331243EE-7953-441B-AED6-9A2C98CDC53C}" name="ID" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5BDFCAEE-0B12-4296-9D05-35A3D489F401}" name="Data35" displayName="Data35" ref="F2:G10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5BDFCAEE-0B12-4296-9D05-35A3D489F401}" name="Data35" displayName="Data35" ref="F2:G10" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="F2:G10" xr:uid="{0025CE4B-7270-49F6-875C-F810B632926D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F3:G10">
     <sortCondition ref="F3:F10"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C23357DE-436E-4EC0-9E05-3208C36EC3C7}" name="Date" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{4A6FF81D-E831-4204-BE03-B858DECC6A19}" name="ID" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C23357DE-436E-4EC0-9E05-3208C36EC3C7}" name="Date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4A6FF81D-E831-4204-BE03-B858DECC6A19}" name="ID" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B6FBBA56-33EA-4B0B-8C64-D7BBD70FFAE2}" name="Data6" displayName="Data6" ref="C2:D10" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="C2:D10" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:D10">
+    <sortCondition ref="C3:C10"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FA88BD5C-5FC9-4F28-AD41-4FDFA8C95B39}" name="Date" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B3E8429A-E7C3-4BDF-99FB-7149C8D83F98}" name="ID" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{024FE4AD-1285-499F-AA30-DCF7EB4BE2E7}" name="Data37" displayName="Data37" ref="F2:G10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+  <autoFilter ref="F2:G10" xr:uid="{0025CE4B-7270-49F6-875C-F810B632926D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F3:G10">
+    <sortCondition ref="F3:F10"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C06B9ACC-AFB6-4F02-AEE4-B11FB3CD3759}" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{CAE0B7AF-FF38-445A-B598-CF6510BA0270}" name="ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1549,6 +1899,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2F65E1F3-0F65-46C0-BFBB-E85D4155B402}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S25"/>
@@ -1567,15 +1944,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="8"/>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="17"/>
       <c r="K1" s="7" t="s">
         <v>17</v>
       </c>
@@ -1799,8 +2176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F57DFC3-7434-48F2-80F5-83E0D3C9E3AE}">
   <dimension ref="B1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1814,16 +2191,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="8"/>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="K1" s="7" t="s">
+      <c r="G1" s="17"/>
+      <c r="K1" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2055,7 +2432,7 @@
       <c r="S11"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.5">
-      <c r="K12" s="14" t="str" cm="1">
+      <c r="K12" s="12" t="str" cm="1">
         <f t="array" ref="K12:L20">_xlfn.LET(
 _xlpm.d, Data4[Date],
 _xlpm.id, Data4[ID],
@@ -2064,15 +2441,15 @@
 )</f>
         <v>Date</v>
       </c>
-      <c r="L12" s="15" t="str">
+      <c r="L12" s="13" t="str">
         <v>ID</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.5">
-      <c r="K13" s="16">
+      <c r="K13" s="14">
         <v>45567</v>
       </c>
-      <c r="L13" s="17" t="str">
+      <c r="L13" s="15" t="str">
         <v>XM-X12</v>
       </c>
       <c r="N13" t="b" cm="1">
@@ -2084,10 +2461,10 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.5">
-      <c r="K14" s="16">
+      <c r="K14" s="14">
         <v>45568</v>
       </c>
-      <c r="L14" s="18" t="str">
+      <c r="L14" s="16" t="str">
         <v>IXM3X</v>
       </c>
       <c r="N14" t="b">
@@ -2098,10 +2475,10 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.5">
-      <c r="K15" s="16">
+      <c r="K15" s="14">
         <v>45569</v>
       </c>
-      <c r="L15" s="18" t="str">
+      <c r="L15" s="16" t="str">
         <v>87X</v>
       </c>
       <c r="N15" t="b">
@@ -2112,10 +2489,10 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.5">
-      <c r="K16" s="16">
+      <c r="K16" s="14">
         <v>45570</v>
       </c>
-      <c r="L16" s="18" t="str">
+      <c r="L16" s="16" t="str">
         <v>X8X9X1</v>
       </c>
       <c r="N16" t="b">
@@ -2126,10 +2503,10 @@
       </c>
     </row>
     <row r="17" spans="11:19" x14ac:dyDescent="0.5">
-      <c r="K17" s="16">
+      <c r="K17" s="14">
         <v>45571</v>
       </c>
-      <c r="L17" s="18" t="str">
+      <c r="L17" s="16" t="str">
         <v>Xmna</v>
       </c>
       <c r="N17" t="b">
@@ -2140,10 +2517,10 @@
       </c>
     </row>
     <row r="18" spans="11:19" x14ac:dyDescent="0.5">
-      <c r="K18" s="16">
+      <c r="K18" s="14">
         <v>45572</v>
       </c>
-      <c r="L18" s="18" t="str">
+      <c r="L18" s="16" t="str">
         <v>XFX</v>
       </c>
       <c r="N18" t="b">
@@ -2154,10 +2531,10 @@
       </c>
     </row>
     <row r="19" spans="11:19" x14ac:dyDescent="0.5">
-      <c r="K19" s="16">
+      <c r="K19" s="14">
         <v>45573</v>
       </c>
-      <c r="L19" s="18" t="str">
+      <c r="L19" s="16" t="str">
         <v>X</v>
       </c>
       <c r="N19" t="b">
@@ -2168,10 +2545,10 @@
       </c>
     </row>
     <row r="20" spans="11:19" x14ac:dyDescent="0.5">
-      <c r="K20" s="16">
+      <c r="K20" s="14">
         <v>45574</v>
       </c>
-      <c r="L20" s="18" t="str">
+      <c r="L20" s="16" t="str">
         <v>R</v>
       </c>
       <c r="N20" t="b">
@@ -2200,6 +2577,295 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="11:19" x14ac:dyDescent="0.5">
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" xr:uid="{AFC8266D-00DE-4448-9E49-ABE3F31F9713}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E915867-6791-43D2-BA34-F0343CA7BDF0}">
+  <dimension ref="B1:S25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="3" max="4" width="12.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="K1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <v>45567</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="9">
+        <v>45567</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C4" s="9">
+        <f t="shared" ref="C4:C10" si="0">C3+1</f>
+        <v>45568</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F10" si="1">F3+1</f>
+        <v>45568</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C5" s="9">
+        <f t="shared" si="0"/>
+        <v>45569</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="9">
+        <f t="shared" si="1"/>
+        <v>45569</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>45570</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="9">
+        <f t="shared" si="1"/>
+        <v>45570</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>45571</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="9">
+        <f t="shared" si="1"/>
+        <v>45571</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>45572</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="9">
+        <f t="shared" si="1"/>
+        <v>45572</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>45573</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="9">
+        <f t="shared" si="1"/>
+        <v>45573</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+    </row>
+    <row r="10" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>45574</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="9">
+        <f t="shared" si="1"/>
+        <v>45574</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="C13" s="4" t="str" cm="1">
+        <f t="array" ref="C13:C20">_xlfn.REDUCE(SUBSTITUTE(D3:D10,"x","X"),{6,4,2,2},_xlfn.LAMBDA(_xlpm.a,_xlpm.x,SUBSTITUTE(_xlpm.a,REPT("X",_xlpm.x),"X")))</f>
+        <v>XM-X12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="C14" s="4" t="str">
+        <v>IXM3X</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="C15" s="4" t="str">
+        <v>87X</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.5">
+      <c r="C16" s="4" t="str">
+        <v>X8X9X1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.5">
+      <c r="C17" s="4" t="str">
+        <v>Xmna</v>
+      </c>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.5">
+      <c r="C18" s="4" t="str">
+        <v>XFX</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.5">
+      <c r="C19" s="4" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.5">
+      <c r="C20" s="4" t="str">
+        <v>R</v>
+      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.5">
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.5">
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.5">
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.5">
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2211,10 +2877,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
   <tableParts count="2">
+    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>